<commit_message>
push of initial steering code
</commit_message>
<xml_diff>
--- a/potenResistanceGraphs.xlsx
+++ b/potenResistanceGraphs.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddiebrower/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maddiebrower/Dropbox/dev/spragueResearch2019/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7F596726-0F3D-6F4B-BF4E-59936CCB5F44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7598AE3-D970-2945-B249-9F3AF959FD6E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="25440" windowHeight="14320" xr2:uid="{1EAE506B-3FA0-B94C-A4CD-10EB782C1EBB}"/>
+    <workbookView xWindow="40" yWindow="460" windowWidth="25440" windowHeight="14320" xr2:uid="{1EAE506B-3FA0-B94C-A4CD-10EB782C1EBB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -211,86 +211,124 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="7.5531077891424075E-2"/>
+                  <c:y val="0.14235268450385768"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$B$2:$B$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>1.3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>2.46</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>3.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>4.75</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>5.37</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>5.52</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>5.89</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$12</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>4</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.4</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.46</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.75</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.37</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.52</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.89</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.9</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -334,57 +372,51 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$12</c:f>
+              <c:f>Sheet1!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>5.94</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>5.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>5.94</c:v>
@@ -405,12 +437,6 @@
                   <c:v>5.94</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.94</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.94</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>5.94</c:v>
                 </c:pt>
               </c:numCache>
@@ -453,86 +479,124 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.2065086081391676E-2"/>
+                  <c:y val="7.5110573394950317E-3"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$2:$A$12</c:f>
+              <c:f>Sheet1!$A$2:$A$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>81</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>108</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>135</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>162</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>216</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
+                  <c:v>243</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$2:$D$12</c:f>
+              <c:f>Sheet1!$D$2:$D$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5.94</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.94</c:v>
+                  <c:v>5.72</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.72</c:v>
+                  <c:v>5.16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.16</c:v>
+                  <c:v>4.5999999999999996</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5999999999999996</c:v>
+                  <c:v>4.0199999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.0199999999999996</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3.12</c:v>
+                  <c:v>2.02</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.02</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0.27700000000000002</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -827,7 +891,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$B$16</c:f>
+              <c:f>Sheet1!$B$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -862,84 +926,72 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:f>Sheet1!$A$15:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$17:$B$27</c:f>
+              <c:f>Sheet1!$B$15:$B$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>2.7</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39</c:v>
+                  <c:v>1.65</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.65</c:v>
+                  <c:v>2.66</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.66</c:v>
+                  <c:v>3.42</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.42</c:v>
+                  <c:v>4.05</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4.05</c:v>
+                  <c:v>4.76</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.76</c:v>
+                  <c:v>5.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.4</c:v>
+                  <c:v>5.48</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.48</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>5.78</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -956,7 +1008,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$16</c:f>
+              <c:f>Sheet1!$C$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -991,52 +1043,46 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:f>Sheet1!$A$15:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$17:$C$27</c:f>
+              <c:f>Sheet1!$C$15:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5.8</c:v>
                 </c:pt>
@@ -1062,12 +1108,6 @@
                   <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.8</c:v>
-                </c:pt>
-                <c:pt idx="10">
                   <c:v>5.8</c:v>
                 </c:pt>
               </c:numCache>
@@ -1085,7 +1125,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$D$16</c:f>
+              <c:f>Sheet1!$D$14</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1120,84 +1160,72 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$17:$A$27</c:f>
+              <c:f>Sheet1!$A$15:$A$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>20</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>30</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>40</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50</c:v>
+                  <c:v>60</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>60</c:v>
+                  <c:v>70</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>70</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>80</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>90</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>100</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$D$17:$D$27</c:f>
+              <c:f>Sheet1!$D$15:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>5.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.8</c:v>
+                  <c:v>5.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.38</c:v>
+                  <c:v>4.84</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.84</c:v>
+                  <c:v>4.3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.3</c:v>
+                  <c:v>3.72</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3.72</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.8</c:v>
+                  <c:v>1.59</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.59</c:v>
+                  <c:v>1.5</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.5</c:v>
-                </c:pt>
-                <c:pt idx="9">
                   <c:v>0.53</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2538,7 +2566,7 @@
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>177800</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>88900</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2568,13 +2596,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>209550</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>654050</xdr:colOff>
-      <xdr:row>29</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>31750</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -2900,10 +2928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F60B58BE-1BFE-4449-8CE6-81AEBBDF3413}">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2924,339 +2952,292 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0</v>
+        <f>270*0.1</f>
+        <v>27</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>0.4</v>
       </c>
       <c r="C2">
-        <v>5.94</v>
+        <v>5.9</v>
       </c>
       <c r="D2">
         <v>5.94</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>10</v>
+        <f>270*0.2</f>
+        <v>54</v>
       </c>
       <c r="B3">
-        <v>0.4</v>
+        <v>1.3</v>
       </c>
       <c r="C3">
-        <v>5.9</v>
+        <v>5.94</v>
       </c>
       <c r="D3">
-        <v>5.94</v>
-      </c>
-      <c r="F3" t="s">
-        <v>4</v>
+        <v>5.72</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>20</v>
+        <f>270*0.3</f>
+        <v>81</v>
       </c>
       <c r="B4">
-        <v>1.3</v>
+        <v>2.46</v>
       </c>
       <c r="C4">
         <v>5.94</v>
       </c>
       <c r="D4">
-        <v>5.72</v>
+        <v>5.16</v>
+      </c>
+      <c r="G4">
+        <f>0.9*270</f>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>30</v>
+        <f>270*0.4</f>
+        <v>108</v>
       </c>
       <c r="B5">
-        <v>2.46</v>
+        <v>3.3</v>
       </c>
       <c r="C5">
         <v>5.94</v>
       </c>
       <c r="D5">
-        <v>5.16</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G5">
-        <f>0.9*270</f>
-        <v>243</v>
+        <f>0.1*270</f>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>40</v>
+        <f>270*0.5</f>
+        <v>135</v>
       </c>
       <c r="B6">
-        <v>3.3</v>
+        <v>4</v>
       </c>
       <c r="C6">
         <v>5.94</v>
       </c>
       <c r="D6">
-        <v>4.5999999999999996</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="G6">
-        <f>0.1*270</f>
-        <v>27</v>
+        <f>243-27</f>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>50</v>
+        <f>270*0.6</f>
+        <v>162</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>4.75</v>
       </c>
       <c r="C7">
         <v>5.94</v>
       </c>
       <c r="D7">
-        <v>4.0199999999999996</v>
-      </c>
-      <c r="G7">
-        <f>243-27</f>
-        <v>216</v>
+        <v>3.12</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>60</v>
+        <f>270*0.7</f>
+        <v>189</v>
       </c>
       <c r="B8">
-        <v>4.75</v>
+        <v>5.37</v>
       </c>
       <c r="C8">
         <v>5.94</v>
       </c>
       <c r="D8">
-        <v>3.12</v>
+        <v>2.02</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>70</v>
+        <f>270*0.8</f>
+        <v>216</v>
       </c>
       <c r="B9">
-        <v>5.37</v>
+        <v>5.52</v>
       </c>
       <c r="C9">
         <v>5.94</v>
       </c>
       <c r="D9">
-        <v>2.02</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>80</v>
+        <f>270*0.9</f>
+        <v>243</v>
       </c>
       <c r="B10">
-        <v>5.52</v>
+        <v>5.89</v>
       </c>
       <c r="C10">
         <v>5.94</v>
       </c>
       <c r="D10">
-        <v>1.5</v>
+        <v>0.27700000000000002</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>90</v>
-      </c>
-      <c r="B11">
-        <v>5.89</v>
-      </c>
-      <c r="C11">
-        <v>5.94</v>
-      </c>
-      <c r="D11">
-        <v>0.27700000000000002</v>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>100</v>
-      </c>
-      <c r="B12">
-        <v>5.9</v>
-      </c>
-      <c r="C12">
-        <v>5.94</v>
-      </c>
-      <c r="D12">
-        <v>5</v>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>0.39</v>
+      </c>
+      <c r="C15">
+        <v>5.8</v>
+      </c>
+      <c r="D15">
+        <v>5.8</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" t="s">
-        <v>3</v>
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16">
+        <v>1.65</v>
+      </c>
+      <c r="C16">
+        <v>5.8</v>
+      </c>
+      <c r="D16">
+        <v>5.38</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B17">
-        <v>2.7</v>
+        <v>2.66</v>
       </c>
       <c r="C17">
         <v>5.8</v>
       </c>
       <c r="D17">
-        <v>5.8</v>
+        <v>4.84</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B18">
-        <v>0.39</v>
+        <v>3.42</v>
       </c>
       <c r="C18">
         <v>5.8</v>
       </c>
       <c r="D18">
-        <v>5.8</v>
+        <v>4.3</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>20</v>
+        <v>50</v>
       </c>
       <c r="B19">
-        <v>1.65</v>
+        <v>4.05</v>
       </c>
       <c r="C19">
         <v>5.8</v>
       </c>
       <c r="D19">
-        <v>5.38</v>
+        <v>3.72</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B20">
-        <v>2.66</v>
+        <v>4.76</v>
       </c>
       <c r="C20">
         <v>5.8</v>
       </c>
       <c r="D20">
-        <v>4.84</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="B21">
-        <v>3.42</v>
+        <v>5.4</v>
       </c>
       <c r="C21">
         <v>5.8</v>
       </c>
       <c r="D21">
-        <v>4.3</v>
+        <v>1.59</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B22">
-        <v>4.05</v>
+        <v>5.48</v>
       </c>
       <c r="C22">
         <v>5.8</v>
       </c>
       <c r="D22">
-        <v>3.72</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>60</v>
+        <v>90</v>
       </c>
       <c r="B23">
-        <v>4.76</v>
+        <v>5.78</v>
       </c>
       <c r="C23">
         <v>5.8</v>
       </c>
       <c r="D23">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>70</v>
-      </c>
-      <c r="B24">
-        <v>5.4</v>
-      </c>
-      <c r="C24">
-        <v>5.8</v>
-      </c>
-      <c r="D24">
-        <v>1.59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>80</v>
-      </c>
-      <c r="B25">
-        <v>5.48</v>
-      </c>
-      <c r="C25">
-        <v>5.8</v>
-      </c>
-      <c r="D25">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A26">
-        <v>90</v>
-      </c>
-      <c r="B26">
-        <v>5.78</v>
-      </c>
-      <c r="C26">
-        <v>5.8</v>
-      </c>
-      <c r="D26">
         <v>0.53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>100</v>
-      </c>
-      <c r="B27">
-        <v>5.8</v>
-      </c>
-      <c r="C27">
-        <v>5.8</v>
-      </c>
-      <c r="D27">
-        <v>3.2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>